<commit_message>
vault backup: 2024-03-14 09:25:42
</commit_message>
<xml_diff>
--- a/tickets/9199134-sharepoint-workflow/workflow-detail.xlsx
+++ b/tickets/9199134-sharepoint-workflow/workflow-detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scwd365-my.sharepoint.com/personal/jlopez_scwd_org/Documents/Documents/FY23/Job Perfomance (Goals &amp; Check-ins)/GOAL #1 - Review Staff Reports/Switch to Teams 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/tickets/9199134-sharepoint-workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="741" documentId="8_{B347893C-FA53-40F5-A6AC-4496ABDBB694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{682F42E4-E136-4F30-B440-4B576F92CF4E}"/>
+  <xr:revisionPtr revIDLastSave="743" documentId="8_{B347893C-FA53-40F5-A6AC-4496ABDBB694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01A2ACB8-A80E-4C32-88F1-CB303EA989EF}"/>
   <bookViews>
-    <workbookView xWindow="29820" yWindow="0" windowWidth="20925" windowHeight="15285" activeTab="1" xr2:uid="{5E6D16AD-E474-4733-8652-063305D65AF0}"/>
+    <workbookView xWindow="28680" yWindow="450" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5E6D16AD-E474-4733-8652-063305D65AF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Teams Folder Mapping" sheetId="1" r:id="rId1"/>
@@ -817,15 +817,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -842,6 +833,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1499,9 +1499,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1539,7 +1539,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1645,7 +1645,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1787,7 +1787,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1821,18 +1821,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2175,7 +2175,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E45" sqref="A1:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,31 +2189,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -2555,11 +2555,11 @@
       <c r="D26" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="2" t="s">
         <v>107</v>
       </c>
@@ -2773,7 +2773,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2845,58 +2845,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="13" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>